<commit_message>
Added category in DocType
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD44034-E97D-4206-B6D5-1A3CAEA4D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5314A7DF-20C2-4F1C-9AB6-F8E91BC140FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$M$268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$N$268</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="735">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2238,6 +2238,69 @@
     <t>cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:digital:ver1.0
 cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:utskrift:ver1.0
 cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:flyttet:ver1.0</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Pre-Award</t>
+  </si>
+  <si>
+    <t>Catalogue</t>
+  </si>
+  <si>
+    <t>Application Response</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Credit Note</t>
+  </si>
+  <si>
+    <t>Order Response</t>
+  </si>
+  <si>
+    <t>Despatch Advice</t>
+  </si>
+  <si>
+    <t>Message Level Response</t>
+  </si>
+  <si>
+    <t>Utility Statement</t>
+  </si>
+  <si>
+    <t>Reminder</t>
+  </si>
+  <si>
+    <t>Invoice Response</t>
+  </si>
+  <si>
+    <t>Catalogue Response</t>
+  </si>
+  <si>
+    <t>Receipt Advice</t>
+  </si>
+  <si>
+    <t>Order Related</t>
+  </si>
+  <si>
+    <t>German Report (old)</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Peppol Network Report</t>
+  </si>
+  <si>
+    <t>HR-XML</t>
+  </si>
+  <si>
+    <t>Digital Post</t>
   </si>
 </sst>
 </file>
@@ -2900,11 +2963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:M268"/>
+  <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M269" sqref="M269"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A268" sqref="A268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,11 +2984,12 @@
     <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="23"/>
     <col min="12" max="12" width="19.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="84.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="5"/>
+    <col min="13" max="13" width="19.140625" style="23" customWidth="1"/>
+    <col min="14" max="14" width="84.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>124</v>
       </c>
@@ -2962,11 +3026,14 @@
       <c r="L1" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>7</v>
       </c>
@@ -2999,11 +3066,14 @@
       <c r="L2" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N2" s="36" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>8</v>
       </c>
@@ -3036,11 +3106,14 @@
       <c r="L3" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N3" s="36" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>9</v>
       </c>
@@ -3073,11 +3146,14 @@
       <c r="L4" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="M4" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N4" s="36" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>100</v>
       </c>
@@ -3110,11 +3186,14 @@
       <c r="L5" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="N5" s="36" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>103</v>
       </c>
@@ -3147,11 +3226,14 @@
       <c r="L6" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="33" t="s">
+        <v>717</v>
+      </c>
+      <c r="N6" s="36" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>103</v>
       </c>
@@ -3184,11 +3266,14 @@
       <c r="L7" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M7" s="36" t="s">
+      <c r="M7" s="33" t="s">
+        <v>717</v>
+      </c>
+      <c r="N7" s="36" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>36</v>
       </c>
@@ -3221,11 +3306,14 @@
       <c r="L8" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="N8" s="36" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>28</v>
       </c>
@@ -3258,11 +3346,14 @@
       <c r="L9" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N9" s="36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>349</v>
       </c>
@@ -3298,11 +3389,14 @@
       <c r="L10" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M10" s="36" t="s">
+      <c r="M10" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N10" s="36" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>29</v>
       </c>
@@ -3335,11 +3429,14 @@
       <c r="L11" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="M11" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N11" s="36" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>25</v>
       </c>
@@ -3372,11 +3469,14 @@
       <c r="L12" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M12" s="36" t="s">
+      <c r="M12" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N12" s="36" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>26</v>
       </c>
@@ -3409,11 +3509,14 @@
       <c r="L13" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M13" s="36" t="s">
+      <c r="M13" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N13" s="36" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>101</v>
       </c>
@@ -3446,11 +3549,14 @@
       <c r="L14" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M14" s="36" t="s">
+      <c r="M14" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N14" s="36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>102</v>
       </c>
@@ -3483,11 +3589,14 @@
       <c r="L15" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M15" s="36" t="s">
+      <c r="M15" s="33" t="s">
+        <v>720</v>
+      </c>
+      <c r="N15" s="36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>101</v>
       </c>
@@ -3520,11 +3629,14 @@
       <c r="L16" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="36" t="s">
+      <c r="M16" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N16" s="36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>91</v>
       </c>
@@ -3557,11 +3669,14 @@
       <c r="L17" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N17" s="36" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>92</v>
       </c>
@@ -3594,11 +3709,14 @@
       <c r="L18" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="33" t="s">
+        <v>720</v>
+      </c>
+      <c r="N18" s="36" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>96</v>
       </c>
@@ -3631,11 +3749,14 @@
       <c r="L19" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M19" s="36" t="s">
+      <c r="M19" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N19" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>97</v>
       </c>
@@ -3668,11 +3789,14 @@
       <c r="L20" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M20" s="36" t="s">
+      <c r="M20" s="33" t="s">
+        <v>721</v>
+      </c>
+      <c r="N20" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>97</v>
       </c>
@@ -3705,11 +3829,14 @@
       <c r="L21" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M21" s="36" t="s">
+      <c r="M21" s="33" t="s">
+        <v>721</v>
+      </c>
+      <c r="N21" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>98</v>
       </c>
@@ -3742,11 +3869,14 @@
       <c r="L22" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N22" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>99</v>
       </c>
@@ -3779,11 +3909,14 @@
       <c r="L23" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M23" s="36" t="s">
+      <c r="M23" s="33" t="s">
+        <v>720</v>
+      </c>
+      <c r="N23" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>98</v>
       </c>
@@ -3816,11 +3949,14 @@
       <c r="L24" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M24" s="36" t="s">
+      <c r="M24" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N24" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
         <v>34</v>
       </c>
@@ -3851,11 +3987,14 @@
       <c r="L25" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M25" s="36" t="s">
+      <c r="M25" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="N25" s="36" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>35</v>
       </c>
@@ -3881,11 +4020,14 @@
       <c r="L26" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N26" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>94</v>
       </c>
@@ -3918,11 +4060,14 @@
       <c r="L27" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M27" s="36" t="s">
+      <c r="M27" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N27" s="36" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>346</v>
       </c>
@@ -3958,11 +4103,14 @@
       <c r="L28" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M28" s="36" t="s">
+      <c r="M28" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N28" s="36" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>95</v>
       </c>
@@ -3995,11 +4143,14 @@
       <c r="L29" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M29" s="36" t="s">
+      <c r="M29" s="33" t="s">
+        <v>721</v>
+      </c>
+      <c r="N29" s="36" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
         <v>39</v>
       </c>
@@ -4032,11 +4183,14 @@
       <c r="L30" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M30" s="36" t="s">
+      <c r="M30" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="N30" s="36" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
         <v>40</v>
       </c>
@@ -4069,11 +4223,14 @@
       <c r="L31" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M31" s="36" t="s">
+      <c r="M31" s="33" t="s">
+        <v>723</v>
+      </c>
+      <c r="N31" s="36" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>468</v>
       </c>
@@ -4102,11 +4259,14 @@
       <c r="L32" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="M32" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N32" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>469</v>
       </c>
@@ -4135,11 +4295,14 @@
       <c r="L33" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M33" s="7" t="s">
+      <c r="M33" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N33" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -4165,11 +4328,14 @@
       <c r="L34" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M34" s="5" t="s">
+      <c r="M34" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N34" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>343</v>
       </c>
@@ -4203,11 +4369,14 @@
       <c r="L35" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M35" s="36" t="s">
+      <c r="M35" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N35" s="36" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>125</v>
       </c>
@@ -4236,11 +4405,14 @@
       <c r="L36" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M36" s="5" t="s">
+      <c r="M36" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N36" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>470</v>
       </c>
@@ -4269,11 +4441,14 @@
       <c r="L37" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="M37" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N37" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
         <v>486</v>
       </c>
@@ -4309,11 +4484,14 @@
       <c r="L38" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M38" s="36" t="s">
+      <c r="M38" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N38" s="36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
         <v>485</v>
       </c>
@@ -4349,11 +4527,14 @@
       <c r="L39" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M39" s="36" t="s">
+      <c r="M39" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N39" s="36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
         <v>484</v>
       </c>
@@ -4389,11 +4570,14 @@
       <c r="L40" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M40" s="36" t="s">
+      <c r="M40" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N40" s="36" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
         <v>483</v>
       </c>
@@ -4429,11 +4613,14 @@
       <c r="L41" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M41" s="36" t="s">
+      <c r="M41" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N41" s="36" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
         <v>482</v>
       </c>
@@ -4469,11 +4656,14 @@
       <c r="L42" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M42" s="36" t="s">
+      <c r="M42" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N42" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="36" t="s">
         <v>481</v>
       </c>
@@ -4509,11 +4699,14 @@
       <c r="L43" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M43" s="36" t="s">
+      <c r="M43" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N43" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>104</v>
       </c>
@@ -4549,11 +4742,14 @@
       <c r="L44" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M44" s="19" t="s">
+      <c r="M44" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N44" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>105</v>
       </c>
@@ -4589,11 +4785,14 @@
       <c r="L45" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M45" s="19" t="s">
+      <c r="M45" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="N45" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>106</v>
       </c>
@@ -4629,11 +4828,14 @@
       <c r="L46" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M46" s="19" t="s">
+      <c r="M46" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N46" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>61</v>
       </c>
@@ -4662,11 +4864,14 @@
       <c r="L47" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M47" s="7" t="s">
+      <c r="M47" s="23" t="s">
+        <v>724</v>
+      </c>
+      <c r="N47" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>62</v>
       </c>
@@ -4695,11 +4900,14 @@
       <c r="L48" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M48" s="7" t="s">
+      <c r="M48" s="23" t="s">
+        <v>725</v>
+      </c>
+      <c r="N48" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>63</v>
       </c>
@@ -4728,11 +4936,14 @@
       <c r="L49" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M49" s="7" t="s">
+      <c r="M49" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N49" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>64</v>
       </c>
@@ -4761,11 +4972,14 @@
       <c r="L50" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M50" s="7" t="s">
+      <c r="M50" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N50" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
         <v>458</v>
       </c>
@@ -4798,11 +5012,14 @@
       <c r="L51" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M51" s="36" t="s">
+      <c r="M51" s="33" t="s">
+        <v>726</v>
+      </c>
+      <c r="N51" s="36" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>459</v>
       </c>
@@ -4831,11 +5048,14 @@
       <c r="L52" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M52" s="5" t="s">
+      <c r="M52" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="N52" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>460</v>
       </c>
@@ -4864,11 +5084,14 @@
       <c r="L53" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M53" s="7" t="s">
+      <c r="M53" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="N53" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>461</v>
       </c>
@@ -4900,11 +5123,14 @@
       <c r="L54" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M54" s="5" t="s">
+      <c r="M54" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N54" s="5" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>462</v>
       </c>
@@ -4933,11 +5159,14 @@
       <c r="L55" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M55" s="7" t="s">
+      <c r="M55" s="23" t="s">
+        <v>726</v>
+      </c>
+      <c r="N55" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>464</v>
       </c>
@@ -4966,11 +5195,14 @@
       <c r="L56" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M56" s="7" t="s">
+      <c r="M56" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="N56" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>463</v>
       </c>
@@ -4999,11 +5231,14 @@
       <c r="L57" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M57" s="7" t="s">
+      <c r="M57" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N57" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>465</v>
       </c>
@@ -5032,11 +5267,14 @@
       <c r="L58" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M58" s="7" t="s">
+      <c r="M58" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="N58" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>466</v>
       </c>
@@ -5065,11 +5303,14 @@
       <c r="L59" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M59" s="7" t="s">
+      <c r="M59" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N59" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>467</v>
       </c>
@@ -5098,11 +5339,14 @@
       <c r="L60" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M60" s="7" t="s">
+      <c r="M60" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="N60" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>79</v>
       </c>
@@ -5128,11 +5372,14 @@
       <c r="L61" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M61" s="7" t="s">
+      <c r="M61" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N61" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>81</v>
       </c>
@@ -5158,11 +5405,14 @@
       <c r="L62" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M62" s="7" t="s">
+      <c r="M62" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N62" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>471</v>
       </c>
@@ -5191,11 +5441,14 @@
       <c r="L63" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M63" s="7" t="s">
+      <c r="M63" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N63" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="36" t="s">
         <v>344</v>
       </c>
@@ -5231,11 +5484,14 @@
       <c r="L64" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M64" s="39" t="s">
+      <c r="M64" s="33" t="s">
+        <v>720</v>
+      </c>
+      <c r="N64" s="39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>472</v>
       </c>
@@ -5267,11 +5523,14 @@
       <c r="L65" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M65" s="7" t="s">
+      <c r="M65" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N65" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>85</v>
       </c>
@@ -5307,11 +5566,14 @@
       <c r="L66" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M66" s="19" t="s">
+      <c r="M66" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N66" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>86</v>
       </c>
@@ -5347,11 +5609,14 @@
       <c r="L67" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M67" s="19" t="s">
+      <c r="M67" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="N67" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>87</v>
       </c>
@@ -5387,11 +5652,14 @@
       <c r="L68" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M68" s="19" t="s">
+      <c r="M68" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N68" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>107</v>
       </c>
@@ -5420,11 +5688,14 @@
       <c r="L69" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M69" s="7" t="s">
+      <c r="M69" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N69" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>108</v>
       </c>
@@ -5453,11 +5724,14 @@
       <c r="L70" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M70" s="7" t="s">
+      <c r="M70" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N70" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>112</v>
       </c>
@@ -5486,11 +5760,14 @@
       <c r="L71" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M71" s="7" t="s">
+      <c r="M71" s="23" t="s">
+        <v>728</v>
+      </c>
+      <c r="N71" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>473</v>
       </c>
@@ -5522,11 +5799,14 @@
       <c r="L72" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M72" s="7" t="s">
+      <c r="M72" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N72" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>474</v>
       </c>
@@ -5558,11 +5838,14 @@
       <c r="L73" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M73" s="7" t="s">
+      <c r="M73" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N73" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>118</v>
       </c>
@@ -5591,11 +5874,14 @@
       <c r="L74" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M74" s="7" t="s">
+      <c r="M74" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N74" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>119</v>
       </c>
@@ -5624,11 +5910,14 @@
       <c r="L75" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M75" s="7" t="s">
+      <c r="M75" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N75" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>161</v>
       </c>
@@ -5664,11 +5953,14 @@
       <c r="L76" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M76" s="19" t="s">
+      <c r="M76" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N76" s="19" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>164</v>
       </c>
@@ -5704,11 +5996,14 @@
       <c r="L77" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M77" s="19" t="s">
+      <c r="M77" s="24" t="s">
+        <v>718</v>
+      </c>
+      <c r="N77" s="19" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>166</v>
       </c>
@@ -5744,11 +6039,14 @@
       <c r="L78" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M78" s="19" t="s">
+      <c r="M78" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N78" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>167</v>
       </c>
@@ -5784,11 +6082,14 @@
       <c r="L79" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M79" s="19" t="s">
+      <c r="M79" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="N79" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>168</v>
       </c>
@@ -5824,11 +6125,14 @@
       <c r="L80" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M80" s="19" t="s">
+      <c r="M80" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N80" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>171</v>
       </c>
@@ -5857,11 +6161,14 @@
       <c r="L81" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M81" s="7" t="s">
+      <c r="M81" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N81" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>172</v>
       </c>
@@ -5890,11 +6197,14 @@
       <c r="L82" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M82" s="7" t="s">
+      <c r="M82" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N82" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>241</v>
       </c>
@@ -5930,11 +6240,14 @@
       <c r="L83" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M83" s="19" t="s">
+      <c r="M83" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N83" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>173</v>
       </c>
@@ -5963,11 +6276,14 @@
       <c r="L84" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M84" s="7" t="s">
+      <c r="M84" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N84" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
         <v>176</v>
       </c>
@@ -6003,11 +6319,14 @@
       <c r="L85" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M85" s="19" t="s">
+      <c r="M85" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N85" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
         <v>177</v>
       </c>
@@ -6043,11 +6362,14 @@
       <c r="L86" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M86" s="19" t="s">
+      <c r="M86" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="N86" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:13" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
         <v>178</v>
       </c>
@@ -6083,11 +6405,14 @@
       <c r="L87" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M87" s="19" t="s">
+      <c r="M87" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N87" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>183</v>
       </c>
@@ -6116,11 +6441,14 @@
       <c r="L88" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M88" s="7" t="s">
+      <c r="M88" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N88" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="36" t="s">
         <v>232</v>
       </c>
@@ -6154,11 +6482,14 @@
       <c r="L89" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M89" s="36" t="s">
+      <c r="M89" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="N89" s="36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:13" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="36" t="s">
         <v>233</v>
       </c>
@@ -6192,11 +6523,14 @@
       <c r="L90" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M90" s="36" t="s">
+      <c r="M90" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="N90" s="36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="36" t="s">
         <v>234</v>
       </c>
@@ -6230,11 +6564,14 @@
       <c r="L91" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M91" s="36" t="s">
+      <c r="M91" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="N91" s="36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="36" t="s">
         <v>235</v>
       </c>
@@ -6268,11 +6605,14 @@
       <c r="L92" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M92" s="36" t="s">
+      <c r="M92" s="33" t="s">
+        <v>721</v>
+      </c>
+      <c r="N92" s="36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>195</v>
       </c>
@@ -6301,11 +6641,14 @@
       <c r="L93" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M93" s="5" t="s">
+      <c r="M93" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N93" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>196</v>
       </c>
@@ -6334,11 +6677,14 @@
       <c r="L94" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M94" s="5" t="s">
+      <c r="M94" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N94" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>197</v>
       </c>
@@ -6367,11 +6713,14 @@
       <c r="L95" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M95" s="5" t="s">
+      <c r="M95" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N95" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>202</v>
       </c>
@@ -6400,11 +6749,14 @@
       <c r="L96" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M96" s="7" t="s">
+      <c r="M96" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N96" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>203</v>
       </c>
@@ -6433,11 +6785,14 @@
       <c r="L97" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M97" s="7" t="s">
+      <c r="M97" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N97" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>245</v>
       </c>
@@ -6473,11 +6828,14 @@
       <c r="L98" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M98" s="19" t="s">
+      <c r="M98" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="N98" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>204</v>
       </c>
@@ -6506,11 +6864,14 @@
       <c r="L99" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M99" s="7" t="s">
+      <c r="M99" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N99" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>221</v>
       </c>
@@ -6539,11 +6900,14 @@
       <c r="L100" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M100" s="5" t="s">
+      <c r="M100" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N100" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>222</v>
       </c>
@@ -6572,11 +6936,14 @@
       <c r="L101" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M101" s="7" t="s">
+      <c r="M101" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N101" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>223</v>
       </c>
@@ -6605,11 +6972,14 @@
       <c r="L102" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M102" s="10" t="s">
+      <c r="M102" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="N102" s="10" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="103" spans="1:13" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
         <v>231</v>
       </c>
@@ -6643,11 +7013,14 @@
       </c>
       <c r="K103" s="24"/>
       <c r="L103" s="24"/>
-      <c r="M103" s="19" t="s">
+      <c r="M103" s="24" t="s">
+        <v>730</v>
+      </c>
+      <c r="N103" s="19" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>184</v>
       </c>
@@ -6676,11 +7049,14 @@
       <c r="L104" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M104" s="5" t="s">
+      <c r="M104" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N104" s="5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>185</v>
       </c>
@@ -6709,11 +7085,14 @@
       <c r="L105" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M105" s="5" t="s">
+      <c r="M105" s="23" t="s">
+        <v>729</v>
+      </c>
+      <c r="N105" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>186</v>
       </c>
@@ -6742,11 +7121,14 @@
       <c r="L106" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M106" s="5" t="s">
+      <c r="M106" s="23" t="s">
+        <v>729</v>
+      </c>
+      <c r="N106" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>187</v>
       </c>
@@ -6775,11 +7157,14 @@
       <c r="L107" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M107" s="5" t="s">
+      <c r="M107" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N107" s="5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>251</v>
       </c>
@@ -6808,11 +7193,14 @@
       <c r="L108" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M108" s="5" t="s">
+      <c r="M108" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N108" s="5" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>252</v>
       </c>
@@ -6841,11 +7229,14 @@
       <c r="L109" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M109" s="5" t="s">
+      <c r="M109" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N109" s="5" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>253</v>
       </c>
@@ -6874,11 +7265,14 @@
       <c r="L110" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M110" s="5" t="s">
+      <c r="M110" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N110" s="5" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>254</v>
       </c>
@@ -6907,11 +7301,14 @@
       <c r="L111" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M111" s="5" t="s">
+      <c r="M111" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N111" s="5" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>255</v>
       </c>
@@ -6940,11 +7337,14 @@
       <c r="L112" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M112" s="5" t="s">
+      <c r="M112" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N112" s="5" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>256</v>
       </c>
@@ -6973,11 +7373,14 @@
       <c r="L113" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M113" s="5" t="s">
+      <c r="M113" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N113" s="5" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>257</v>
       </c>
@@ -7006,11 +7409,14 @@
       <c r="L114" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M114" s="5" t="s">
+      <c r="M114" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N114" s="5" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>258</v>
       </c>
@@ -7039,11 +7445,14 @@
       <c r="L115" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M115" s="5" t="s">
+      <c r="M115" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N115" s="5" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>259</v>
       </c>
@@ -7072,11 +7481,14 @@
       <c r="L116" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M116" s="5" t="s">
+      <c r="M116" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N116" s="5" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>260</v>
       </c>
@@ -7105,11 +7517,14 @@
       <c r="L117" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M117" s="5" t="s">
+      <c r="M117" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N117" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>261</v>
       </c>
@@ -7138,11 +7553,14 @@
       <c r="L118" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M118" s="5" t="s">
+      <c r="M118" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N118" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>262</v>
       </c>
@@ -7171,11 +7589,14 @@
       <c r="L119" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M119" s="5" t="s">
+      <c r="M119" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N119" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>263</v>
       </c>
@@ -7204,11 +7625,14 @@
       <c r="L120" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M120" s="5" t="s">
+      <c r="M120" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N120" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>264</v>
       </c>
@@ -7237,11 +7661,14 @@
       <c r="L121" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M121" s="5" t="s">
+      <c r="M121" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N121" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>265</v>
       </c>
@@ -7270,11 +7697,14 @@
       <c r="L122" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M122" s="5" t="s">
+      <c r="M122" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N122" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>266</v>
       </c>
@@ -7303,11 +7733,14 @@
       <c r="L123" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M123" s="5" t="s">
+      <c r="M123" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N123" s="5" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>267</v>
       </c>
@@ -7336,11 +7769,14 @@
       <c r="L124" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M124" s="5" t="s">
+      <c r="M124" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N124" s="5" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>268</v>
       </c>
@@ -7369,11 +7805,14 @@
       <c r="L125" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M125" s="5" t="s">
+      <c r="M125" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N125" s="5" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>269</v>
       </c>
@@ -7402,11 +7841,14 @@
       <c r="L126" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M126" s="5" t="s">
+      <c r="M126" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N126" s="5" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>270</v>
       </c>
@@ -7435,11 +7877,14 @@
       <c r="L127" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M127" s="5" t="s">
+      <c r="M127" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N127" s="5" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>271</v>
       </c>
@@ -7468,11 +7913,14 @@
       <c r="L128" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M128" s="5" t="s">
+      <c r="M128" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N128" s="5" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>272</v>
       </c>
@@ -7501,11 +7949,14 @@
       <c r="L129" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="M129" s="5" t="s">
+      <c r="M129" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="N129" s="5" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>475</v>
       </c>
@@ -7536,11 +7987,14 @@
       <c r="L130" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M130" s="5" t="s">
+      <c r="M130" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N130" s="5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>476</v>
       </c>
@@ -7571,11 +8025,14 @@
       <c r="L131" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M131" s="5" t="s">
+      <c r="M131" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N131" s="5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>477</v>
       </c>
@@ -7606,11 +8063,14 @@
       <c r="L132" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M132" s="5" t="s">
+      <c r="M132" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N132" s="5" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>478</v>
       </c>
@@ -7641,11 +8101,14 @@
       <c r="L133" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M133" s="5" t="s">
+      <c r="M133" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N133" s="5" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>305</v>
       </c>
@@ -7673,11 +8136,14 @@
       <c r="L134" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M134" s="5" t="s">
+      <c r="M134" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="N134" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>306</v>
       </c>
@@ -7705,11 +8171,14 @@
       <c r="L135" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M135" s="5" t="s">
+      <c r="M135" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="N135" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>307</v>
       </c>
@@ -7737,11 +8206,14 @@
       <c r="L136" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M136" s="5" t="s">
+      <c r="M136" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N136" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>308</v>
       </c>
@@ -7769,11 +8241,14 @@
       <c r="L137" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M137" s="5" t="s">
+      <c r="M137" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N137" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>309</v>
       </c>
@@ -7801,11 +8276,14 @@
       <c r="L138" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M138" s="5" t="s">
+      <c r="M138" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="N138" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>310</v>
       </c>
@@ -7833,11 +8311,14 @@
       <c r="L139" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M139" s="5" t="s">
+      <c r="M139" s="23" t="s">
+        <v>725</v>
+      </c>
+      <c r="N139" s="5" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>311</v>
       </c>
@@ -7865,11 +8346,14 @@
       <c r="L140" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M140" s="5" t="s">
+      <c r="M140" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="N140" s="5" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>312</v>
       </c>
@@ -7897,11 +8381,14 @@
       <c r="L141" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M141" s="5" t="s">
+      <c r="M141" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="N141" s="5" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>313</v>
       </c>
@@ -7929,11 +8416,14 @@
       <c r="L142" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M142" s="5" t="s">
+      <c r="M142" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N142" s="5" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>314</v>
       </c>
@@ -7961,11 +8451,14 @@
       <c r="L143" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M143" s="5" t="s">
+      <c r="M143" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="N143" s="5" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>315</v>
       </c>
@@ -7993,11 +8486,14 @@
       <c r="L144" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M144" s="5" t="s">
+      <c r="M144" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N144" s="5" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>316</v>
       </c>
@@ -8025,11 +8521,14 @@
       <c r="L145" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M145" s="5" t="s">
+      <c r="M145" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N145" s="5" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>317</v>
       </c>
@@ -8057,11 +8556,14 @@
       <c r="L146" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M146" s="5" t="s">
+      <c r="M146" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N146" s="5" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>318</v>
       </c>
@@ -8089,11 +8591,14 @@
       <c r="L147" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M147" s="5" t="s">
+      <c r="M147" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N147" s="5" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>350</v>
       </c>
@@ -8121,11 +8626,14 @@
       <c r="L148" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M148" s="7" t="s">
+      <c r="M148" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N148" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>351</v>
       </c>
@@ -8153,11 +8661,14 @@
       <c r="L149" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M149" s="7" t="s">
+      <c r="M149" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N149" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>352</v>
       </c>
@@ -8185,11 +8696,14 @@
       <c r="L150" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M150" s="7" t="s">
+      <c r="M150" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N150" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>357</v>
       </c>
@@ -8217,11 +8731,14 @@
       <c r="L151" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M151" s="7" t="s">
+      <c r="M151" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N151" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>358</v>
       </c>
@@ -8249,11 +8766,14 @@
       <c r="L152" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M152" s="7" t="s">
+      <c r="M152" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N152" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>359</v>
       </c>
@@ -8281,11 +8801,14 @@
       <c r="L153" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M153" s="7" t="s">
+      <c r="M153" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N153" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>375</v>
       </c>
@@ -8313,11 +8836,14 @@
       <c r="L154" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M154" s="5" t="s">
+      <c r="M154" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N154" s="5" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>376</v>
       </c>
@@ -8345,11 +8871,14 @@
       <c r="L155" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M155" s="5" t="s">
+      <c r="M155" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N155" s="5" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>377</v>
       </c>
@@ -8377,11 +8906,14 @@
       <c r="L156" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M156" s="5" t="s">
+      <c r="M156" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N156" s="5" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>389</v>
       </c>
@@ -8412,11 +8944,14 @@
       <c r="L157" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M157" s="5" t="s">
+      <c r="M157" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N157" s="5" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>390</v>
       </c>
@@ -8447,11 +8982,14 @@
       <c r="L158" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M158" s="5" t="s">
+      <c r="M158" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N158" s="5" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>391</v>
       </c>
@@ -8482,11 +9020,14 @@
       <c r="L159" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M159" s="5" t="s">
+      <c r="M159" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N159" s="5" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>392</v>
       </c>
@@ -8517,11 +9058,14 @@
       <c r="L160" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M160" s="5" t="s">
+      <c r="M160" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N160" s="5" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>393</v>
       </c>
@@ -8552,11 +9096,14 @@
       <c r="L161" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M161" s="5" t="s">
+      <c r="M161" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N161" s="5" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>394</v>
       </c>
@@ -8587,11 +9134,14 @@
       <c r="L162" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M162" s="5" t="s">
+      <c r="M162" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N162" s="5" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>395</v>
       </c>
@@ -8622,11 +9172,14 @@
       <c r="L163" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M163" s="5" t="s">
+      <c r="M163" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N163" s="5" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>396</v>
       </c>
@@ -8657,11 +9210,14 @@
       <c r="L164" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M164" s="5" t="s">
+      <c r="M164" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N164" s="5" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>397</v>
       </c>
@@ -8692,11 +9248,14 @@
       <c r="L165" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M165" s="5" t="s">
+      <c r="M165" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N165" s="5" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>398</v>
       </c>
@@ -8727,11 +9286,14 @@
       <c r="L166" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M166" s="5" t="s">
+      <c r="M166" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N166" s="5" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>399</v>
       </c>
@@ -8762,11 +9324,14 @@
       <c r="L167" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M167" s="5" t="s">
+      <c r="M167" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N167" s="5" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>400</v>
       </c>
@@ -8797,11 +9362,14 @@
       <c r="L168" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M168" s="5" t="s">
+      <c r="M168" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N168" s="5" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>401</v>
       </c>
@@ -8832,11 +9400,14 @@
       <c r="L169" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M169" s="5" t="s">
+      <c r="M169" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N169" s="5" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>402</v>
       </c>
@@ -8867,11 +9438,14 @@
       <c r="L170" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M170" s="5" t="s">
+      <c r="M170" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N170" s="5" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>405</v>
       </c>
@@ -8902,11 +9476,14 @@
       <c r="L171" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M171" s="5" t="s">
+      <c r="M171" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N171" s="5" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>404</v>
       </c>
@@ -8937,11 +9514,14 @@
       <c r="L172" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M172" s="5" t="s">
+      <c r="M172" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N172" s="5" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="173" spans="1:13" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A173" s="36" t="s">
         <v>564</v>
       </c>
@@ -8976,11 +9556,14 @@
       <c r="L173" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M173" s="36" t="s">
+      <c r="M173" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="N173" s="36" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>403</v>
       </c>
@@ -9011,11 +9594,14 @@
       <c r="L174" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M174" s="5" t="s">
+      <c r="M174" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N174" s="5" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>427</v>
       </c>
@@ -9043,11 +9629,14 @@
       <c r="L175" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M175" s="7" t="s">
+      <c r="M175" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N175" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>428</v>
       </c>
@@ -9075,11 +9664,14 @@
       <c r="L176" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M176" s="7" t="s">
+      <c r="M176" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N176" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>429</v>
       </c>
@@ -9107,11 +9699,14 @@
       <c r="L177" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M177" s="7" t="s">
+      <c r="M177" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N177" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>430</v>
       </c>
@@ -9139,11 +9734,14 @@
       <c r="L178" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M178" s="7" t="s">
+      <c r="M178" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N178" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>431</v>
       </c>
@@ -9171,11 +9769,14 @@
       <c r="L179" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M179" s="7" t="s">
+      <c r="M179" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N179" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>432</v>
       </c>
@@ -9203,11 +9804,14 @@
       <c r="L180" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M180" s="7" t="s">
+      <c r="M180" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N180" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="181" spans="1:13" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="36" t="s">
         <v>479</v>
       </c>
@@ -9240,11 +9844,14 @@
       <c r="L181" s="33" t="s">
         <v>444</v>
       </c>
-      <c r="M181" s="36" t="s">
+      <c r="M181" s="33" t="s">
+        <v>732</v>
+      </c>
+      <c r="N181" s="36" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="182" spans="1:13" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="36" t="s">
         <v>480</v>
       </c>
@@ -9277,11 +9884,14 @@
       <c r="L182" s="33" t="s">
         <v>444</v>
       </c>
-      <c r="M182" s="36" t="s">
+      <c r="M182" s="33" t="s">
+        <v>732</v>
+      </c>
+      <c r="N182" s="36" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>574</v>
       </c>
@@ -9312,11 +9922,14 @@
       <c r="L183" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M183" s="43" t="s">
+      <c r="M183" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N183" s="43" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>575</v>
       </c>
@@ -9347,11 +9960,14 @@
       <c r="L184" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M184" s="14" t="s">
+      <c r="M184" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N184" s="14" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>576</v>
       </c>
@@ -9382,11 +9998,14 @@
       <c r="L185" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M185" s="14" t="s">
+      <c r="M185" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N185" s="14" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>453</v>
       </c>
@@ -9414,11 +10033,14 @@
       <c r="L186" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M186" s="5" t="s">
+      <c r="M186" s="23" t="s">
+        <v>724</v>
+      </c>
+      <c r="N186" s="5" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>487</v>
       </c>
@@ -9446,11 +10068,14 @@
       <c r="L187" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M187" s="5" t="s">
+      <c r="M187" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N187" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>490</v>
       </c>
@@ -9488,11 +10113,14 @@
       <c r="L188" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M188" s="7" t="s">
+      <c r="M188" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N188" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>498</v>
       </c>
@@ -9523,11 +10151,14 @@
       <c r="L189" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M189" s="5" t="s">
+      <c r="M189" s="23" t="s">
+        <v>729</v>
+      </c>
+      <c r="N189" s="5" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>499</v>
       </c>
@@ -9558,11 +10189,14 @@
       <c r="L190" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M190" s="5" t="s">
+      <c r="M190" s="23" t="s">
+        <v>729</v>
+      </c>
+      <c r="N190" s="5" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>500</v>
       </c>
@@ -9593,11 +10227,14 @@
       <c r="L191" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M191" s="5" t="s">
+      <c r="M191" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="N191" s="5" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>514</v>
       </c>
@@ -9625,11 +10262,14 @@
       <c r="L192" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M192" s="7" t="s">
+      <c r="M192" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N192" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>515</v>
       </c>
@@ -9657,11 +10297,14 @@
       <c r="L193" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M193" s="7" t="s">
+      <c r="M193" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N193" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>516</v>
       </c>
@@ -9689,11 +10332,14 @@
       <c r="L194" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M194" s="7" t="s">
+      <c r="M194" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N194" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>517</v>
       </c>
@@ -9721,11 +10367,14 @@
       <c r="L195" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M195" s="7" t="s">
+      <c r="M195" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N195" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>518</v>
       </c>
@@ -9753,11 +10402,14 @@
       <c r="L196" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M196" s="7" t="s">
+      <c r="M196" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N196" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>519</v>
       </c>
@@ -9785,11 +10437,14 @@
       <c r="L197" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M197" s="7" t="s">
+      <c r="M197" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N197" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="198" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>526</v>
       </c>
@@ -9827,11 +10482,14 @@
       <c r="L198" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M198" s="7" t="s">
+      <c r="M198" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N198" s="7" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>530</v>
       </c>
@@ -9863,11 +10521,14 @@
       <c r="L199" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M199" s="5" t="s">
+      <c r="M199" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N199" s="5" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>531</v>
       </c>
@@ -9899,11 +10560,14 @@
       <c r="L200" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M200" s="5" t="s">
+      <c r="M200" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N200" s="5" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>535</v>
       </c>
@@ -9935,11 +10599,14 @@
       <c r="L201" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M201" s="5" t="s">
+      <c r="M201" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N201" s="5" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>536</v>
       </c>
@@ -9971,11 +10638,14 @@
       <c r="L202" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M202" s="5" t="s">
+      <c r="M202" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N202" s="5" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>540</v>
       </c>
@@ -10006,11 +10676,14 @@
       <c r="L203" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M203" s="5" t="s">
+      <c r="M203" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N203" s="5" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="204" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>541</v>
       </c>
@@ -10041,11 +10714,14 @@
       <c r="L204" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M204" s="5" t="s">
+      <c r="M204" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N204" s="5" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>545</v>
       </c>
@@ -10076,11 +10752,14 @@
       <c r="L205" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M205" s="5" t="s">
+      <c r="M205" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N205" s="5" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>546</v>
       </c>
@@ -10111,11 +10790,14 @@
       <c r="L206" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M206" s="5" t="s">
+      <c r="M206" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N206" s="5" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>551</v>
       </c>
@@ -10146,11 +10828,14 @@
       <c r="L207" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M207" s="5" t="s">
+      <c r="M207" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N207" s="5" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>550</v>
       </c>
@@ -10181,11 +10866,14 @@
       <c r="L208" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M208" s="5" t="s">
+      <c r="M208" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N208" s="5" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>555</v>
       </c>
@@ -10216,11 +10904,14 @@
       <c r="L209" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M209" s="5" t="s">
+      <c r="M209" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N209" s="5" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>556</v>
       </c>
@@ -10251,11 +10942,14 @@
       <c r="L210" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M210" s="5" t="s">
+      <c r="M210" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N210" s="5" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>566</v>
       </c>
@@ -10286,11 +10980,14 @@
       <c r="L211" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M211" s="5" t="s">
+      <c r="M211" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N211" s="5" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="212" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>568</v>
       </c>
@@ -10321,11 +11018,14 @@
       <c r="L212" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M212" s="5" t="s">
+      <c r="M212" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N212" s="5" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="213" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>569</v>
       </c>
@@ -10356,11 +11056,14 @@
       <c r="L213" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="M213" s="5" t="s">
+      <c r="M213" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N213" s="5" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>578</v>
       </c>
@@ -10391,11 +11094,14 @@
       <c r="L214" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M214" s="42" t="s">
+      <c r="M214" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N214" s="42" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>579</v>
       </c>
@@ -10426,11 +11132,14 @@
       <c r="L215" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M215" s="42" t="s">
+      <c r="M215" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N215" s="42" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="216" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>580</v>
       </c>
@@ -10461,11 +11170,14 @@
       <c r="L216" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M216" s="42" t="s">
+      <c r="M216" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N216" s="42" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>581</v>
       </c>
@@ -10496,11 +11208,14 @@
       <c r="L217" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M217" s="42" t="s">
+      <c r="M217" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N217" s="42" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>582</v>
       </c>
@@ -10531,11 +11246,14 @@
       <c r="L218" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M218" s="42" t="s">
+      <c r="M218" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N218" s="42" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="219" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>583</v>
       </c>
@@ -10566,11 +11284,14 @@
       <c r="L219" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="M219" s="42" t="s">
+      <c r="M219" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="N219" s="42" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>598</v>
       </c>
@@ -10598,11 +11319,14 @@
       <c r="L220" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M220" s="5" t="s">
+      <c r="M220" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N220" s="5" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>603</v>
       </c>
@@ -10630,11 +11354,14 @@
       <c r="L221" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="M221" s="5" t="s">
+      <c r="M221" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="N221" s="5" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>604</v>
       </c>
@@ -10662,11 +11389,14 @@
       <c r="L222" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="M222" s="5" t="s">
+      <c r="M222" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="N222" s="5" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>614</v>
       </c>
@@ -10697,11 +11427,14 @@
       <c r="L223" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M223" s="5" t="s">
+      <c r="M223" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N223" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>615</v>
       </c>
@@ -10732,11 +11465,14 @@
       <c r="L224" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M224" s="5" t="s">
+      <c r="M224" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N224" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>618</v>
       </c>
@@ -10773,11 +11509,14 @@
       <c r="L225" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M225" s="5" t="s">
+      <c r="M225" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N225" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>618</v>
       </c>
@@ -10808,11 +11547,14 @@
       <c r="L226" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M226" s="5" t="s">
+      <c r="M226" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N226" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>526</v>
       </c>
@@ -10843,11 +11585,14 @@
       <c r="L227" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M227" s="5" t="s">
+      <c r="M227" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N227" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>619</v>
       </c>
@@ -10884,11 +11629,14 @@
       <c r="L228" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M228" s="5" t="s">
+      <c r="M228" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N228" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>619</v>
       </c>
@@ -10919,11 +11667,14 @@
       <c r="L229" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M229" s="5" t="s">
+      <c r="M229" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N229" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>621</v>
       </c>
@@ -10954,11 +11705,14 @@
       <c r="L230" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M230" s="5" t="s">
+      <c r="M230" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N230" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="231" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>623</v>
       </c>
@@ -10989,11 +11743,14 @@
       <c r="L231" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M231" s="5" t="s">
+      <c r="M231" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N231" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>625</v>
       </c>
@@ -11024,11 +11781,14 @@
       <c r="L232" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M232" s="5" t="s">
+      <c r="M232" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N232" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>627</v>
       </c>
@@ -11059,11 +11819,14 @@
       <c r="L233" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M233" s="5" t="s">
+      <c r="M233" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N233" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>621</v>
       </c>
@@ -11094,11 +11857,14 @@
       <c r="L234" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M234" s="5" t="s">
+      <c r="M234" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N234" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="235" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>623</v>
       </c>
@@ -11129,11 +11895,14 @@
       <c r="L235" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M235" s="5" t="s">
+      <c r="M235" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N235" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>625</v>
       </c>
@@ -11164,11 +11933,14 @@
       <c r="L236" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M236" s="5" t="s">
+      <c r="M236" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N236" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>627</v>
       </c>
@@ -11199,11 +11971,14 @@
       <c r="L237" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M237" s="5" t="s">
+      <c r="M237" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N237" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="238" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>632</v>
       </c>
@@ -11231,11 +12006,14 @@
       <c r="L238" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M238" s="7" t="s">
+      <c r="M238" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N238" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="239" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>633</v>
       </c>
@@ -11263,11 +12041,14 @@
       <c r="L239" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M239" s="7" t="s">
+      <c r="M239" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N239" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="240" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>634</v>
       </c>
@@ -11295,11 +12076,14 @@
       <c r="L240" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M240" s="7" t="s">
+      <c r="M240" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N240" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="241" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>635</v>
       </c>
@@ -11327,11 +12111,14 @@
       <c r="L241" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M241" s="7" t="s">
+      <c r="M241" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N241" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
         <v>636</v>
       </c>
@@ -11359,11 +12146,14 @@
       <c r="L242" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M242" s="7" t="s">
+      <c r="M242" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N242" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="243" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
         <v>637</v>
       </c>
@@ -11391,11 +12181,14 @@
       <c r="L243" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M243" s="7" t="s">
+      <c r="M243" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N243" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
         <v>647</v>
       </c>
@@ -11426,11 +12219,14 @@
       <c r="L244" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M244" s="5" t="s">
+      <c r="M244" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N244" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
         <v>646</v>
       </c>
@@ -11461,11 +12257,14 @@
       <c r="L245" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M245" s="5" t="s">
+      <c r="M245" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N245" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>658</v>
       </c>
@@ -11496,11 +12295,14 @@
       <c r="L246" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M246" s="5" t="s">
+      <c r="M246" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N246" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="247" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>659</v>
       </c>
@@ -11531,11 +12333,14 @@
       <c r="L247" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M247" s="5" t="s">
+      <c r="M247" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N247" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>660</v>
       </c>
@@ -11566,11 +12371,14 @@
       <c r="L248" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M248" s="5" t="s">
+      <c r="M248" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N248" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="249" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>661</v>
       </c>
@@ -11601,11 +12409,14 @@
       <c r="L249" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M249" s="5" t="s">
+      <c r="M249" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N249" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>658</v>
       </c>
@@ -11636,11 +12447,14 @@
       <c r="L250" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M250" s="5" t="s">
+      <c r="M250" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N250" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>659</v>
       </c>
@@ -11671,11 +12485,14 @@
       <c r="L251" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M251" s="5" t="s">
+      <c r="M251" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N251" s="5" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>660</v>
       </c>
@@ -11706,11 +12523,14 @@
       <c r="L252" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M252" s="5" t="s">
+      <c r="M252" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N252" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="253" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>661</v>
       </c>
@@ -11741,11 +12561,14 @@
       <c r="L253" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="M253" s="5" t="s">
+      <c r="M253" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="N253" s="5" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
         <v>669</v>
       </c>
@@ -11773,11 +12596,14 @@
       <c r="L254" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M254" s="5" t="s">
+      <c r="M254" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N254" s="5" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
         <v>674</v>
       </c>
@@ -11805,11 +12631,14 @@
       <c r="L255" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M255" s="5" t="s">
+      <c r="M255" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N255" s="5" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
         <v>675</v>
       </c>
@@ -11837,11 +12666,14 @@
       <c r="L256" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M256" s="5" t="s">
+      <c r="M256" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N256" s="5" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" s="5" t="s">
         <v>677</v>
       </c>
@@ -11869,11 +12701,14 @@
       <c r="L257" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M257" s="5" t="s">
+      <c r="M257" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N257" s="5" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
         <v>678</v>
       </c>
@@ -11901,11 +12736,14 @@
       <c r="L258" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M258" s="5" t="s">
+      <c r="M258" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N258" s="5" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259" s="5" t="s">
         <v>680</v>
       </c>
@@ -11933,11 +12771,14 @@
       <c r="L259" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M259" s="5" t="s">
+      <c r="M259" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="N259" s="5" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="260" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
         <v>697</v>
       </c>
@@ -11965,11 +12806,14 @@
       <c r="L260" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M260" s="5" t="s">
+      <c r="M260" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N260" s="5" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="261" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
         <v>698</v>
       </c>
@@ -11997,11 +12841,14 @@
       <c r="L261" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M261" s="5" t="s">
+      <c r="M261" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N261" s="5" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="262" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
         <v>699</v>
       </c>
@@ -12029,11 +12876,14 @@
       <c r="L262" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M262" s="5" t="s">
+      <c r="M262" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N262" s="5" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="263" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
         <v>700</v>
       </c>
@@ -12061,11 +12911,14 @@
       <c r="L263" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M263" s="5" t="s">
+      <c r="M263" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N263" s="5" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="264" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
         <v>701</v>
       </c>
@@ -12093,11 +12946,14 @@
       <c r="L264" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M264" s="5" t="s">
+      <c r="M264" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N264" s="5" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="265" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="5" t="s">
         <v>702</v>
       </c>
@@ -12125,11 +12981,14 @@
       <c r="L265" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M265" s="5" t="s">
+      <c r="M265" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N265" s="5" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="266" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
         <v>703</v>
       </c>
@@ -12157,11 +13016,14 @@
       <c r="L266" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M266" s="5" t="s">
+      <c r="M266" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N266" s="5" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="267" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="5" t="s">
         <v>704</v>
       </c>
@@ -12189,11 +13051,14 @@
       <c r="L267" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M267" s="5" t="s">
+      <c r="M267" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N267" s="5" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="268" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
         <v>705</v>
       </c>
@@ -12221,12 +13086,15 @@
       <c r="L268" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="M268" s="5" t="s">
+      <c r="M268" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="N268" s="5" t="s">
         <v>711</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M268" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N268" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Marked entries effectively "Removed"
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5314A7DF-20C2-4F1C-9AB6-F8E91BC140FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60055284-812C-441A-9EBB-FE23ECFBFE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2547,9 +2547,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2966,8 +2964,8 @@
   <dimension ref="A1:N268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A268" sqref="A268"/>
+      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A269" sqref="A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10075,48 +10073,48 @@
         <v>130</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="188" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="44" t="s">
         <v>490</v>
       </c>
-      <c r="B188" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C188" s="5" t="s">
+      <c r="B188" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C188" s="15" t="s">
         <v>491</v>
       </c>
-      <c r="D188" s="27" t="s">
+      <c r="D188" s="29" t="s">
         <v>455</v>
       </c>
-      <c r="E188" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="F188" s="44" t="s">
+      <c r="E188" s="24" t="s">
+        <v>502</v>
+      </c>
+      <c r="F188" s="21" t="s">
         <v>670</v>
       </c>
-      <c r="G188" s="13">
+      <c r="G188" s="18">
         <v>45565</v>
       </c>
-      <c r="H188" s="5" t="s">
+      <c r="H188" s="15" t="s">
         <v>707</v>
       </c>
-      <c r="I188" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J188" s="5" t="b">
+      <c r="I188" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J188" s="15" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K188" s="23">
+      <c r="K188" s="24">
         <v>3</v>
       </c>
-      <c r="L188" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="M188" s="23" t="s">
+      <c r="L188" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M188" s="24" t="s">
         <v>719</v>
       </c>
-      <c r="N188" s="7" t="s">
+      <c r="N188" s="19" t="s">
         <v>130</v>
       </c>
     </row>
@@ -10444,48 +10442,48 @@
         <v>130</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="198" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="44" t="s">
         <v>526</v>
       </c>
-      <c r="B198" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C198" s="5" t="s">
+      <c r="B198" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C198" s="15" t="s">
         <v>527</v>
       </c>
-      <c r="D198" s="27" t="s">
+      <c r="D198" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="E198" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="F198" s="44" t="s">
+      <c r="E198" s="24" t="s">
+        <v>502</v>
+      </c>
+      <c r="F198" s="21" t="s">
         <v>670</v>
       </c>
-      <c r="G198" s="13">
+      <c r="G198" s="18">
         <v>45565</v>
       </c>
-      <c r="H198" s="5" t="s">
+      <c r="H198" s="15" t="s">
         <v>708</v>
       </c>
-      <c r="I198" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J198" s="5" t="b">
+      <c r="I198" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J198" s="15" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K198" s="23">
+      <c r="K198" s="24">
         <v>3</v>
       </c>
-      <c r="L198" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="M198" s="23" t="s">
+      <c r="L198" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M198" s="24" t="s">
         <v>719</v>
       </c>
-      <c r="N198" s="7" t="s">
+      <c r="N198" s="19" t="s">
         <v>529</v>
       </c>
     </row>
@@ -11472,47 +11470,47 @@
         <v>613</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+    <row r="225" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A225" s="44" t="s">
         <v>618</v>
       </c>
-      <c r="B225" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C225" s="5" t="s">
+      <c r="B225" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C225" s="15" t="s">
         <v>617</v>
       </c>
-      <c r="D225" s="27" t="s">
+      <c r="D225" s="29" t="s">
         <v>591</v>
       </c>
-      <c r="E225" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="F225" s="44" t="s">
+      <c r="E225" s="24" t="s">
+        <v>502</v>
+      </c>
+      <c r="F225" s="21" t="s">
         <v>670</v>
       </c>
-      <c r="G225" s="13">
+      <c r="G225" s="18">
         <v>45565</v>
       </c>
-      <c r="H225" s="5" t="s">
+      <c r="H225" s="15" t="s">
         <v>709</v>
       </c>
-      <c r="I225" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J225" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K225" s="23">
+      <c r="I225" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J225" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K225" s="24">
         <v>3</v>
       </c>
-      <c r="L225" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="M225" s="23" t="s">
+      <c r="L225" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M225" s="24" t="s">
         <v>719</v>
       </c>
-      <c r="N225" s="5" t="s">
+      <c r="N225" s="15" t="s">
         <v>613</v>
       </c>
     </row>
@@ -11592,47 +11590,47 @@
         <v>529</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+    <row r="228" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A228" s="44" t="s">
         <v>619</v>
       </c>
-      <c r="B228" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C228" s="5" t="s">
+      <c r="B228" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C228" s="15" t="s">
         <v>620</v>
       </c>
-      <c r="D228" s="27" t="s">
+      <c r="D228" s="29" t="s">
         <v>591</v>
       </c>
-      <c r="E228" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="F228" s="44" t="s">
+      <c r="E228" s="24" t="s">
+        <v>502</v>
+      </c>
+      <c r="F228" s="21" t="s">
         <v>670</v>
       </c>
-      <c r="G228" s="13">
+      <c r="G228" s="18">
         <v>45565</v>
       </c>
-      <c r="H228" s="5" t="s">
+      <c r="H228" s="15" t="s">
         <v>709</v>
       </c>
-      <c r="I228" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J228" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K228" s="23">
+      <c r="I228" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J228" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K228" s="24">
         <v>3</v>
       </c>
-      <c r="L228" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="M228" s="23" t="s">
+      <c r="L228" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M228" s="24" t="s">
         <v>719</v>
       </c>
-      <c r="N228" s="5" t="s">
+      <c r="N228" s="15" t="s">
         <v>613</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added "DICO Maintenance Instruction"; TICC-300
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F4CFC1-A3A3-4089-95BD-56A488E44042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3300EE97-3720-4B22-B084-C50F5D6B27E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="746">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2319,6 +2319,21 @@
   </si>
   <si>
     <t>TICC-359</t>
+  </si>
+  <si>
+    <t>http://www.ketenstandaard.nl/onderhoudsopdracht/SALES/005::MaintenanceInstruction##dico:maintenanceinstruction@nl-1.0::1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:dico:2018:maintenance:1.0</t>
+  </si>
+  <si>
+    <t>DICO Maintenance Instruction</t>
+  </si>
+  <si>
+    <t>TICC-300</t>
+  </si>
+  <si>
+    <t>DICO</t>
   </si>
 </sst>
 </file>
@@ -2979,11 +2994,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N270"/>
+  <dimension ref="A1:N271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B271" sqref="B271"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13187,6 +13202,41 @@
         <v>247</v>
       </c>
     </row>
+    <row r="271" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A271" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="D271" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E271" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H271" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="I271" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J271" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L271" s="23" t="s">
+        <v>602</v>
+      </c>
+      <c r="M271" s="23" t="s">
+        <v>745</v>
+      </c>
+      <c r="N271" s="5" t="s">
+        <v>742</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N268" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added "DICO Maintenance Status"; TICC-360
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3300EE97-3720-4B22-B084-C50F5D6B27E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188DFD61-1A24-4C63-9DDB-7132C07679A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="749">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2334,6 +2334,15 @@
   </si>
   <si>
     <t>DICO</t>
+  </si>
+  <si>
+    <t>http://www.ketenstandaard.nl/onderhoudsstatus/SALES/005::MaintenanceStatus##dico:maintenancestatus@nl-1.0::1.0</t>
+  </si>
+  <si>
+    <t>DICO Maintenance Status</t>
+  </si>
+  <si>
+    <t>TICC-360</t>
   </si>
 </sst>
 </file>
@@ -2994,7 +3003,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N271"/>
+  <dimension ref="A1:N272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
@@ -13237,6 +13246,41 @@
         <v>742</v>
       </c>
     </row>
+    <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A272" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="D272" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E272" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H272" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="I272" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J272" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L272" s="23" t="s">
+        <v>602</v>
+      </c>
+      <c r="M272" s="23" t="s">
+        <v>745</v>
+      </c>
+      <c r="N272" s="5" t="s">
+        <v>742</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N268" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added France identifiers; TICC-363
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D93DF6-27D1-44F5-8C7F-98E2E3E59692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7475BB25-7EA9-4125-948E-DDD93032B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="761">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2334,6 +2334,52 @@
   </si>
   <si>
     <t>DICO</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:pdf+xml##urn:cen.eu:en16931:2017#conformant#urn:peppol:france:billing:Factur-X:1.0::D22B</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:france:billing:regulated
+cenbii-procid-ubl::urn:peppol:france:billing:non-regulated</t>
+  </si>
+  <si>
+    <t>POAC-France</t>
+  </si>
+  <si>
+    <t>TICC-363</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:peppol:france:billing:cius:1.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:peppol:france:billing:extended:1.0::2.1</t>
+  </si>
+  <si>
+    <t>France UBL Invoice CIUS</t>
+  </si>
+  <si>
+    <t>France UBL Invoice Extension</t>
+  </si>
+  <si>
+    <t>France CII Invoice CIUS</t>
+  </si>
+  <si>
+    <t>France CII Invoice Extension</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:peppol:france:billing:cius:1.0::D16B</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#conformant#urn:peppol:france:billing:extended:1.0::D22B</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossDomainAcknowledgementAndResponse:100::CrossDomainAcknowledgementAndResponse##urn:peppol:france:billing:cdv:1.0::D22B</t>
+  </si>
+  <si>
+    <t>France Factur-X</t>
+  </si>
+  <si>
+    <t>France CDAR</t>
   </si>
 </sst>
 </file>
@@ -2994,11 +3040,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N272"/>
+  <dimension ref="A1:N277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A272" sqref="A272:XFD272"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A274" sqref="A274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13237,8 +13283,221 @@
         <v>742</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B272" s="4"/>
+    <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A272" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="D272" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E272" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H272" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I272" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J272" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L272" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="M272" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N272" s="5" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="273" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A273" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C273" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="D273" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E273" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H273" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I273" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J273" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L273" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="M273" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N273" s="5" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A274" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="D274" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E274" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H274" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I274" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J274" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L274" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="M274" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N274" s="5" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A275" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C275" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="D275" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E275" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H275" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I275" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J275" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L275" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="M275" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N275" s="5" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A276" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C276" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="D276" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E276" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H276" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I276" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J276" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L276" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="M276" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N276" s="5" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="277" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A277" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="B277" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C277" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="D277" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="E277" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H277" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I277" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J277" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L277" s="23" t="s">
+        <v>748</v>
+      </c>
+      <c r="M277" s="23" t="s">
+        <v>726</v>
+      </c>
+      <c r="N277" s="5" t="s">
+        <v>747</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N268" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Change as requested by FR
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7475BB25-7EA9-4125-948E-DDD93032B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A65184B-5BD4-458D-89B4-235DD661044B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2367,9 +2367,6 @@
     <t>France CII Invoice Extension</t>
   </si>
   <si>
-    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:peppol:france:billing:cius:1.0::D16B</t>
-  </si>
-  <si>
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#conformant#urn:peppol:france:billing:extended:1.0::D22B</t>
   </si>
   <si>
@@ -2380,6 +2377,9 @@
   </si>
   <si>
     <t>France CDAR</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:peppol:france:billing:cius:1.0::D22B</t>
   </si>
 </sst>
 </file>
@@ -3044,7 +3044,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A274" sqref="A274"/>
+      <selection pane="bottomLeft" activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13285,7 +13285,7 @@
     </row>
     <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B272" s="4" t="s">
         <v>56</v>
@@ -13399,7 +13399,7 @@
         <v>56</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="D275" s="27" t="s">
         <v>739</v>
@@ -13435,7 +13435,7 @@
         <v>56</v>
       </c>
       <c r="C276" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D276" s="27" t="s">
         <v>739</v>
@@ -13465,13 +13465,13 @@
     </row>
     <row r="277" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B277" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D277" s="27" t="s">
         <v>739</v>

</xml_diff>

<commit_message>
Added support non-XML document types
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A65184B-5BD4-458D-89B4-235DD661044B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B927724-3F1F-4D90-85D1-E21E56A9ED45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3044,7 +3044,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C276" sqref="C276"/>
+      <selection pane="bottomLeft" activeCell="A277" sqref="A277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13309,6 +13309,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="K272" s="23">
+        <v>1</v>
+      </c>
       <c r="L272" s="23" t="s">
         <v>748</v>
       </c>
@@ -13345,6 +13348,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="K273" s="23">
+        <v>1</v>
+      </c>
       <c r="L273" s="23" t="s">
         <v>748</v>
       </c>
@@ -13381,6 +13387,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="K274" s="23">
+        <v>1</v>
+      </c>
       <c r="L274" s="23" t="s">
         <v>748</v>
       </c>
@@ -13417,6 +13426,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="K275" s="23">
+        <v>1</v>
+      </c>
       <c r="L275" s="23" t="s">
         <v>748</v>
       </c>
@@ -13453,6 +13465,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="K276" s="23">
+        <v>1</v>
+      </c>
       <c r="L276" s="23" t="s">
         <v>748</v>
       </c>
@@ -13487,6 +13502,9 @@
       </c>
       <c r="J277" s="5" t="b">
         <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K277" s="23">
         <v>1</v>
       </c>
       <c r="L277" s="23" t="s">

</xml_diff>